<commit_message>
update Day5, RX/TX OK
</commit_message>
<xml_diff>
--- a/docs/Cogen_Protocol.xlsx
+++ b/docs/Cogen_Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\sim-tools\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711508C5-C194-4BE8-98A5-CB07EE5E8D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C49A60-3A91-45CA-9F93-A4A428EF7261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2769" yWindow="3643" windowWidth="24840" windowHeight="10766" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me" sheetId="11" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="483">
   <si>
     <t>Cogen B'd 제어 로직</t>
     <phoneticPr fontId="21" type="noConversion"/>
@@ -1568,9 +1568,6 @@
     <t>FCid</t>
   </si>
   <si>
-    <t>FCid~Data</t>
-  </si>
-  <si>
     <t>사용 안함</t>
   </si>
   <si>
@@ -1667,9 +1664,6 @@
     <t>제어명령</t>
   </si>
   <si>
-    <t>동작상태</t>
-  </si>
-  <si>
     <t>FW_VER</t>
   </si>
   <si>
@@ -1853,10 +1847,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Addr(</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>Fcid</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -1986,6 +1976,24 @@
   </si>
   <si>
     <t>txdata3</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>COGEN 상태</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>swtCogenSysRun4</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>swtCogenSysRun5</t>
+  </si>
+  <si>
+    <t>swtCogenSysRun6</t>
+  </si>
+  <si>
+    <t>STX~Data</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -3702,7 +3710,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4313,12 +4321,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="40" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8588,8 +8590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B028B19-B245-4EE1-9453-ED4D46D927D6}">
   <dimension ref="B2:W79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="H2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
@@ -8600,7 +8602,7 @@
     <col min="11" max="11" width="11.640625" style="69" customWidth="1"/>
     <col min="12" max="12" width="29.140625" style="69" customWidth="1"/>
     <col min="13" max="19" width="9.140625" style="69"/>
-    <col min="20" max="20" width="10.85546875" style="69" customWidth="1"/>
+    <col min="20" max="20" width="15.0703125" style="69" customWidth="1"/>
     <col min="21" max="21" width="14" style="69" customWidth="1"/>
     <col min="22" max="16384" width="9.140625" style="69"/>
   </cols>
@@ -8633,10 +8635,10 @@
         <v>348</v>
       </c>
       <c r="C3" s="80" t="s">
-        <v>447</v>
+        <v>288</v>
       </c>
       <c r="D3" s="80" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E3" s="80" t="s">
         <v>289</v>
@@ -8683,7 +8685,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="101" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E4" s="66">
         <v>24</v>
@@ -8711,17 +8713,17 @@
       <c r="P4" s="66">
         <v>4</v>
       </c>
-      <c r="Q4" s="207" t="s">
-        <v>474</v>
-      </c>
-      <c r="R4" s="207" t="s">
+      <c r="Q4" s="205" t="s">
+        <v>471</v>
+      </c>
+      <c r="R4" s="205" t="s">
+        <v>361</v>
+      </c>
+      <c r="S4" s="205" t="s">
         <v>362</v>
       </c>
-      <c r="S4" s="207" t="s">
-        <v>363</v>
-      </c>
-      <c r="T4" s="208" t="s">
-        <v>475</v>
+      <c r="T4" s="206" t="s">
+        <v>472</v>
       </c>
       <c r="U4" s="72" t="s">
         <v>345</v>
@@ -8732,16 +8734,16 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.55000000000000004">
       <c r="E5" s="96" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F5" s="73" t="s">
         <v>333</v>
       </c>
       <c r="G5" s="81" t="s">
-        <v>360</v>
-      </c>
-      <c r="U5" s="73" t="s">
-        <v>360</v>
+        <v>482</v>
+      </c>
+      <c r="U5" s="96" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.55000000000000004">
@@ -8749,10 +8751,10 @@
         <v>340</v>
       </c>
       <c r="L7" s="87" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="P7" s="177" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q7" s="177"/>
       <c r="R7" s="177"/>
@@ -8777,13 +8779,13 @@
       </c>
       <c r="H8" s="180"/>
       <c r="I8" s="84" t="s">
+        <v>371</v>
+      </c>
+      <c r="J8" s="84" t="s">
         <v>372</v>
       </c>
-      <c r="J8" s="84" t="s">
-        <v>373</v>
-      </c>
       <c r="L8" s="85" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M8" s="91" t="s">
         <v>347</v>
@@ -8795,16 +8797,16 @@
         <v>350</v>
       </c>
       <c r="P8" s="180" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="Q8" s="180"/>
       <c r="R8" s="180"/>
       <c r="S8" s="180"/>
       <c r="T8" s="84" t="s">
+        <v>371</v>
+      </c>
+      <c r="U8" s="84" t="s">
         <v>372</v>
-      </c>
-      <c r="U8" s="84" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.55000000000000004">
@@ -8824,17 +8826,17 @@
       <c r="G9" s="181"/>
       <c r="H9" s="181"/>
       <c r="I9" s="97" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="J9" s="99" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="L9" s="67"/>
-      <c r="M9" s="209" t="s">
-        <v>474</v>
+      <c r="M9" s="207" t="s">
+        <v>471</v>
       </c>
       <c r="N9" s="67" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O9" s="66">
         <v>0</v>
@@ -8846,10 +8848,10 @@
       <c r="R9" s="181"/>
       <c r="S9" s="181"/>
       <c r="T9" s="67" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="U9" s="99" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.55000000000000004">
@@ -8867,7 +8869,7 @@
       <c r="I10" s="67"/>
       <c r="J10" s="68"/>
       <c r="L10" s="67" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="M10" s="67"/>
       <c r="N10" s="67"/>
@@ -8881,10 +8883,10 @@
       <c r="R10" s="181"/>
       <c r="S10" s="181"/>
       <c r="T10" s="67" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="U10" s="99" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.55000000000000004">
@@ -8904,10 +8906,10 @@
       <c r="G11" s="181"/>
       <c r="H11" s="181"/>
       <c r="I11" s="97" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="J11" s="99" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="L11" s="67"/>
       <c r="M11" s="67"/>
@@ -8916,16 +8918,16 @@
         <v>2</v>
       </c>
       <c r="P11" s="182" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="Q11" s="181"/>
       <c r="R11" s="181"/>
       <c r="S11" s="181"/>
       <c r="T11" s="67" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="U11" s="99" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.55000000000000004">
@@ -8943,7 +8945,7 @@
       <c r="I12" s="67"/>
       <c r="J12" s="68"/>
       <c r="L12" s="67" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="M12" s="67"/>
       <c r="N12" s="67"/>
@@ -8951,16 +8953,16 @@
         <v>3</v>
       </c>
       <c r="P12" s="182" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="Q12" s="181"/>
       <c r="R12" s="181"/>
       <c r="S12" s="181"/>
       <c r="T12" s="67" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="U12" s="99" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.55000000000000004">
@@ -8990,35 +8992,35 @@
         <v>4</v>
       </c>
       <c r="P13" s="189" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="Q13" s="189"/>
       <c r="R13" s="189"/>
       <c r="S13" s="189"/>
       <c r="T13" s="94" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="U13" s="99" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="W13" s="69" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="66">
         <v>5</v>
       </c>
-      <c r="C14" s="211" t="s">
-        <v>478</v>
+      <c r="C14" s="209" t="s">
+        <v>475</v>
       </c>
       <c r="D14" s="185"/>
       <c r="E14" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F14" s="68"/>
       <c r="G14" s="181" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H14" s="181"/>
       <c r="I14" s="83"/>
@@ -9030,16 +9032,16 @@
         <v>5</v>
       </c>
       <c r="P14" s="190" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="Q14" s="191"/>
       <c r="R14" s="191"/>
       <c r="S14" s="191"/>
       <c r="T14" s="67" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="U14" s="99" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.55000000000000004">
@@ -9059,13 +9061,13 @@
       <c r="G15" s="181"/>
       <c r="H15" s="181"/>
       <c r="I15" s="67" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J15" s="99" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="L15" s="98" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="M15" s="67"/>
       <c r="N15" s="67"/>
@@ -9088,17 +9090,17 @@
       </c>
       <c r="D16" s="195"/>
       <c r="E16" s="82" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F16" s="68"/>
       <c r="G16" s="181" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H16" s="181"/>
       <c r="I16" s="83"/>
       <c r="J16" s="100"/>
       <c r="L16" s="98" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="M16" s="67"/>
       <c r="N16" s="67"/>
@@ -9106,7 +9108,7 @@
         <v>7</v>
       </c>
       <c r="P16" s="192" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="Q16" s="193"/>
       <c r="R16" s="193"/>
@@ -9123,23 +9125,23 @@
       </c>
       <c r="D17" s="195"/>
       <c r="E17" s="82" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F17" s="68"/>
       <c r="G17" s="181" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H17" s="181"/>
       <c r="I17" s="83"/>
       <c r="J17" s="100"/>
       <c r="L17" s="67" t="s">
-        <v>421</v>
-      </c>
-      <c r="M17" s="209" t="s">
-        <v>476</v>
+        <v>419</v>
+      </c>
+      <c r="M17" s="207" t="s">
+        <v>473</v>
       </c>
       <c r="N17" s="67" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O17" s="66">
         <v>0</v>
@@ -9151,22 +9153,22 @@
       <c r="R17" s="181"/>
       <c r="S17" s="181"/>
       <c r="T17" s="67" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="U17" s="99" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="66">
         <v>9</v>
       </c>
-      <c r="C18" s="211" t="s">
-        <v>479</v>
+      <c r="C18" s="209" t="s">
+        <v>476</v>
       </c>
       <c r="D18" s="185"/>
       <c r="E18" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F18" s="68"/>
       <c r="G18" s="181"/>
@@ -9180,16 +9182,16 @@
         <v>1</v>
       </c>
       <c r="P18" s="181" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Q18" s="181"/>
       <c r="R18" s="181"/>
       <c r="S18" s="181"/>
       <c r="T18" s="67" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="U18" s="99" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9209,13 +9211,13 @@
       <c r="G19" s="181"/>
       <c r="H19" s="181"/>
       <c r="I19" s="97" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="J19" s="99" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="L19" s="67" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="M19" s="67"/>
       <c r="N19" s="67"/>
@@ -9229,10 +9231,10 @@
       <c r="R19" s="181"/>
       <c r="S19" s="181"/>
       <c r="T19" s="67" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="U19" s="99" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9250,7 +9252,7 @@
       <c r="I20" s="67"/>
       <c r="J20" s="68"/>
       <c r="L20" s="94" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="M20" s="67"/>
       <c r="N20" s="67"/>
@@ -9258,16 +9260,16 @@
         <v>3</v>
       </c>
       <c r="P20" s="181" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q20" s="181"/>
       <c r="R20" s="181"/>
       <c r="S20" s="181"/>
       <c r="T20" s="67" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="U20" s="99" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9287,10 +9289,10 @@
       <c r="G21" s="181"/>
       <c r="H21" s="181"/>
       <c r="I21" s="97" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="J21" s="99" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="L21" s="67"/>
       <c r="M21" s="67"/>
@@ -9305,10 +9307,10 @@
       <c r="R21" s="181"/>
       <c r="S21" s="181"/>
       <c r="T21" s="67" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="U21" s="99" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9326,7 +9328,7 @@
       <c r="I22" s="67"/>
       <c r="J22" s="68"/>
       <c r="L22" s="94" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="M22" s="67"/>
       <c r="N22" s="67"/>
@@ -9340,10 +9342,10 @@
       <c r="R22" s="181"/>
       <c r="S22" s="181"/>
       <c r="T22" s="67" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="U22" s="99" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9355,17 +9357,17 @@
       </c>
       <c r="D23" s="195"/>
       <c r="E23" s="82" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F23" s="68"/>
       <c r="G23" s="181" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H23" s="181"/>
       <c r="I23" s="83"/>
       <c r="J23" s="100"/>
       <c r="L23" s="94" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="M23" s="67"/>
       <c r="N23" s="67"/>
@@ -9379,10 +9381,10 @@
       <c r="R23" s="181"/>
       <c r="S23" s="181"/>
       <c r="T23" s="67" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="U23" s="99" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9404,13 +9406,13 @@
       </c>
       <c r="H24" s="181"/>
       <c r="I24" s="97" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="J24" s="99" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="L24" s="94" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="M24" s="67"/>
       <c r="N24" s="67"/>
@@ -9424,10 +9426,10 @@
       <c r="R24" s="181"/>
       <c r="S24" s="181"/>
       <c r="T24" s="67" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="U24" s="99" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9445,8 +9447,8 @@
       <c r="I25" s="67"/>
       <c r="J25" s="68"/>
       <c r="L25" s="67"/>
-      <c r="M25" s="209" t="s">
-        <v>477</v>
+      <c r="M25" s="207" t="s">
+        <v>474</v>
       </c>
       <c r="N25" s="67" t="s">
         <v>339</v>
@@ -9461,10 +9463,10 @@
       <c r="R25" s="181"/>
       <c r="S25" s="181"/>
       <c r="T25" s="67" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="U25" s="99" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9482,25 +9484,25 @@
         <v>341</v>
       </c>
       <c r="G26" s="182" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H26" s="181"/>
       <c r="I26" s="97" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J26" s="99" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="L26" s="83"/>
-      <c r="M26" s="210" t="s">
-        <v>475</v>
+      <c r="M26" s="208" t="s">
+        <v>472</v>
       </c>
       <c r="N26" s="83" t="s">
         <v>339</v>
       </c>
       <c r="O26" s="83"/>
       <c r="P26" s="184" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q26" s="184"/>
       <c r="R26" s="184"/>
@@ -9527,8 +9529,8 @@
       <c r="B28" s="66">
         <v>19</v>
       </c>
-      <c r="C28" s="211" t="s">
-        <v>480</v>
+      <c r="C28" s="209" t="s">
+        <v>477</v>
       </c>
       <c r="D28" s="185"/>
       <c r="E28" s="1" t="s">
@@ -9559,14 +9561,14 @@
         <v>341</v>
       </c>
       <c r="G29" s="182" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H29" s="181"/>
       <c r="I29" s="97" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="J29" s="99" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.55000000000000004">
@@ -9629,10 +9631,10 @@
       </c>
       <c r="H31" s="181"/>
       <c r="I31" s="97" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J31" s="99" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="M31" s="71" t="s">
         <v>310</v>
@@ -9706,7 +9708,7 @@
     </row>
     <row r="33" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" s="95" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="M33" s="71"/>
       <c r="V33" s="70"/>
@@ -9722,7 +9724,7 @@
     </row>
     <row r="35" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="F35" s="177" t="s">
-        <v>393</v>
+        <v>478</v>
       </c>
       <c r="G35" s="177"/>
       <c r="H35" s="177"/>
@@ -9745,15 +9747,15 @@
         <v>350</v>
       </c>
       <c r="F36" s="178" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G36" s="203"/>
       <c r="H36" s="179"/>
       <c r="I36" s="84" t="s">
+        <v>371</v>
+      </c>
+      <c r="J36" s="84" t="s">
         <v>372</v>
-      </c>
-      <c r="J36" s="84" t="s">
-        <v>373</v>
       </c>
       <c r="M36" s="74" t="s">
         <v>319</v>
@@ -9772,17 +9774,17 @@
     </row>
     <row r="37" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C37" s="92" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D37" s="67" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E37" s="66">
         <v>0</v>
       </c>
-      <c r="F37" s="204"/>
-      <c r="G37" s="205"/>
-      <c r="H37" s="205"/>
+      <c r="F37" s="197"/>
+      <c r="G37" s="198"/>
+      <c r="H37" s="198"/>
       <c r="I37" s="67"/>
       <c r="J37" s="68"/>
     </row>
@@ -9792,13 +9794,13 @@
       <c r="E38" s="66">
         <v>1</v>
       </c>
-      <c r="F38" s="204" t="s">
+      <c r="F38" s="197" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="205"/>
-      <c r="H38" s="205"/>
+      <c r="G38" s="198"/>
+      <c r="H38" s="198"/>
       <c r="I38" s="67" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="J38" s="68"/>
     </row>
@@ -9808,9 +9810,9 @@
       <c r="E39" s="66">
         <v>2</v>
       </c>
-      <c r="F39" s="204"/>
-      <c r="G39" s="205"/>
-      <c r="H39" s="205"/>
+      <c r="F39" s="197"/>
+      <c r="G39" s="198"/>
+      <c r="H39" s="198"/>
       <c r="I39" s="67"/>
       <c r="J39" s="68"/>
     </row>
@@ -9820,11 +9822,11 @@
       <c r="E40" s="66">
         <v>3</v>
       </c>
-      <c r="F40" s="204" t="s">
+      <c r="F40" s="197" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="205"/>
-      <c r="H40" s="205"/>
+      <c r="G40" s="198"/>
+      <c r="H40" s="198"/>
       <c r="I40" s="67" t="s">
         <v>15</v>
       </c>
@@ -9844,10 +9846,10 @@
       <c r="S40" s="183"/>
       <c r="T40" s="73"/>
       <c r="U40" s="89" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="V40" s="89" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="41" spans="3:22" x14ac:dyDescent="0.55000000000000004">
@@ -9856,11 +9858,11 @@
       <c r="E41" s="66">
         <v>4</v>
       </c>
-      <c r="F41" s="204" t="s">
+      <c r="F41" s="197" t="s">
         <v>21</v>
       </c>
-      <c r="G41" s="205"/>
-      <c r="H41" s="205"/>
+      <c r="G41" s="198"/>
+      <c r="H41" s="198"/>
       <c r="I41" s="67" t="s">
         <v>19</v>
       </c>
@@ -9890,9 +9892,9 @@
       <c r="E42" s="66">
         <v>5</v>
       </c>
-      <c r="F42" s="204"/>
-      <c r="G42" s="205"/>
-      <c r="H42" s="205"/>
+      <c r="F42" s="197"/>
+      <c r="G42" s="198"/>
+      <c r="H42" s="198"/>
       <c r="I42" s="67"/>
       <c r="J42" s="68"/>
       <c r="M42" s="116" t="s">
@@ -9920,9 +9922,9 @@
       <c r="E43" s="66">
         <v>6</v>
       </c>
-      <c r="F43" s="204"/>
-      <c r="G43" s="205"/>
-      <c r="H43" s="205"/>
+      <c r="F43" s="197"/>
+      <c r="G43" s="198"/>
+      <c r="H43" s="198"/>
       <c r="I43" s="67"/>
       <c r="J43" s="68"/>
       <c r="M43" s="116" t="s">
@@ -9950,9 +9952,9 @@
       <c r="E44" s="66">
         <v>7</v>
       </c>
-      <c r="F44" s="204"/>
-      <c r="G44" s="205"/>
-      <c r="H44" s="205"/>
+      <c r="F44" s="197"/>
+      <c r="G44" s="198"/>
+      <c r="H44" s="198"/>
       <c r="I44" s="67"/>
       <c r="J44" s="68"/>
       <c r="M44" s="116" t="s">
@@ -9976,17 +9978,17 @@
     </row>
     <row r="45" spans="3:22" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" s="92" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D45" s="67" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E45" s="66">
         <v>0</v>
       </c>
-      <c r="F45" s="204"/>
-      <c r="G45" s="205"/>
-      <c r="H45" s="205"/>
+      <c r="F45" s="197"/>
+      <c r="G45" s="198"/>
+      <c r="H45" s="198"/>
       <c r="I45" s="67"/>
       <c r="J45" s="68"/>
       <c r="M45" s="116" t="s">
@@ -10014,13 +10016,13 @@
       <c r="E46" s="66">
         <v>1</v>
       </c>
-      <c r="F46" s="204" t="s">
-        <v>381</v>
-      </c>
-      <c r="G46" s="205"/>
-      <c r="H46" s="205"/>
+      <c r="F46" s="197" t="s">
+        <v>380</v>
+      </c>
+      <c r="G46" s="198"/>
+      <c r="H46" s="198"/>
       <c r="I46" s="67" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J46" s="68"/>
       <c r="M46" s="116" t="s">
@@ -10049,7 +10051,7 @@
         <v>2</v>
       </c>
       <c r="F47" s="201" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G47" s="202"/>
       <c r="H47" s="202"/>
@@ -10078,12 +10080,12 @@
         <v>3</v>
       </c>
       <c r="F48" s="197" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G48" s="198"/>
       <c r="H48" s="198"/>
       <c r="I48" s="67" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J48" s="68"/>
       <c r="M48" s="116" t="s">
@@ -10109,12 +10111,12 @@
         <v>4</v>
       </c>
       <c r="F49" s="197" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G49" s="198"/>
       <c r="H49" s="198"/>
       <c r="I49" s="67" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J49" s="68"/>
     </row>
@@ -10142,7 +10144,7 @@
       <c r="I51" s="67"/>
       <c r="J51" s="68"/>
       <c r="M51" s="88" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="3:19" x14ac:dyDescent="0.55000000000000004">
@@ -10157,11 +10159,11 @@
       <c r="I52" s="67"/>
       <c r="J52" s="68"/>
       <c r="M52" s="183" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="N52" s="183"/>
       <c r="O52" s="183" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="P52" s="183"/>
       <c r="Q52" s="183" t="s">
@@ -10172,10 +10174,10 @@
     </row>
     <row r="53" spans="3:19" x14ac:dyDescent="0.55000000000000004">
       <c r="C53" s="92" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D53" s="67" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E53" s="66">
         <v>0</v>
@@ -10186,7 +10188,7 @@
       <c r="G53" s="198"/>
       <c r="H53" s="198"/>
       <c r="I53" s="67" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J53" s="68"/>
       <c r="M53" s="116"/>
@@ -10196,7 +10198,7 @@
       </c>
       <c r="P53" s="116"/>
       <c r="Q53" s="128" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="R53" s="128"/>
       <c r="S53" s="128"/>
@@ -10213,7 +10215,7 @@
       <c r="G54" s="198"/>
       <c r="H54" s="198"/>
       <c r="I54" s="67" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J54" s="68"/>
       <c r="M54" s="116"/>
@@ -10221,7 +10223,7 @@
       <c r="O54" s="116"/>
       <c r="P54" s="116"/>
       <c r="Q54" s="128" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="R54" s="128"/>
       <c r="S54" s="128"/>
@@ -10233,12 +10235,12 @@
         <v>2</v>
       </c>
       <c r="F55" s="199" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G55" s="200"/>
       <c r="H55" s="200"/>
       <c r="I55" s="67" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J55" s="68"/>
       <c r="M55" s="116"/>
@@ -10246,7 +10248,7 @@
       <c r="O55" s="116"/>
       <c r="P55" s="116"/>
       <c r="Q55" s="128" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="R55" s="128"/>
       <c r="S55" s="128"/>
@@ -10263,10 +10265,10 @@
       <c r="G56" s="198"/>
       <c r="H56" s="198"/>
       <c r="I56" s="67" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J56" s="68"/>
-      <c r="K56" s="206"/>
+      <c r="K56" s="204"/>
       <c r="M56" s="116"/>
       <c r="N56" s="116"/>
       <c r="O56" s="116"/>
@@ -10287,10 +10289,10 @@
       <c r="G57" s="198"/>
       <c r="H57" s="198"/>
       <c r="I57" s="67" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J57" s="68"/>
-      <c r="K57" s="206"/>
+      <c r="K57" s="204"/>
       <c r="M57" s="116"/>
       <c r="N57" s="116"/>
       <c r="O57" s="116"/>
@@ -10306,15 +10308,17 @@
         <v>5</v>
       </c>
       <c r="F58" s="197" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G58" s="198"/>
       <c r="H58" s="198"/>
       <c r="I58" s="94" t="s">
-        <v>387</v>
-      </c>
-      <c r="J58" s="68"/>
-      <c r="K58" s="206"/>
+        <v>386</v>
+      </c>
+      <c r="J58" s="99" t="s">
+        <v>479</v>
+      </c>
+      <c r="K58" s="204"/>
       <c r="M58" s="116"/>
       <c r="N58" s="116"/>
       <c r="O58" s="116"/>
@@ -10330,15 +10334,17 @@
         <v>6</v>
       </c>
       <c r="F59" s="197" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G59" s="198"/>
       <c r="H59" s="198"/>
       <c r="I59" s="94" t="s">
-        <v>388</v>
-      </c>
-      <c r="J59" s="68"/>
-      <c r="K59" s="206"/>
+        <v>387</v>
+      </c>
+      <c r="J59" s="99" t="s">
+        <v>480</v>
+      </c>
+      <c r="K59" s="204"/>
       <c r="M59" s="116"/>
       <c r="N59" s="116"/>
       <c r="O59" s="116"/>
@@ -10354,15 +10360,17 @@
         <v>7</v>
       </c>
       <c r="F60" s="197" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G60" s="198"/>
       <c r="H60" s="198"/>
       <c r="I60" s="94" t="s">
-        <v>389</v>
-      </c>
-      <c r="J60" s="68"/>
-      <c r="K60" s="206"/>
+        <v>388</v>
+      </c>
+      <c r="J60" s="99" t="s">
+        <v>481</v>
+      </c>
+      <c r="K60" s="204"/>
       <c r="M60" s="116"/>
       <c r="N60" s="116"/>
       <c r="O60" s="116"/>
@@ -10396,13 +10404,7 @@
       <c r="U79" s="73"/>
     </row>
   </sheetData>
-  <mergeCells count="140">
-    <mergeCell ref="F41:H41"/>
-    <mergeCell ref="F42:H42"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="F46:H46"/>
+  <mergeCells count="130">
     <mergeCell ref="M53:N53"/>
     <mergeCell ref="O53:P53"/>
     <mergeCell ref="Q53:S53"/>
@@ -10511,10 +10513,6 @@
     <mergeCell ref="P9:S9"/>
     <mergeCell ref="F35:H35"/>
     <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
     <mergeCell ref="M55:N55"/>
     <mergeCell ref="O55:P55"/>
     <mergeCell ref="Q55:S55"/>

</xml_diff>